<commit_message>
v6 alg is better
</commit_message>
<xml_diff>
--- a/4x4x4solver_v7/analytics.xlsx
+++ b/4x4x4solver_v7/analytics.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\Solvour\4x4x4solver_v7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0EA9C9-2521-4766-B2C9-53876DFFB5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C1399C-FDDC-4513-A9D4-33A9C0F8E3A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4C9BF6D-CD2A-436C-9DDB-5BAD8A64124A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v6" sheetId="3" r:id="rId1"/>
+    <sheet name="phase0改変" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
   <si>
     <t>時間</t>
     <rPh sb="0" eb="2">
@@ -314,7 +315,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$10</c:f>
+              <c:f>'v6'!$F$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -335,7 +336,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$D$11:$D$28</c:f>
+              <c:f>'v6'!$D$11:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -398,36 +399,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$F$28</c:f>
+              <c:f>'v6'!$F$11:$F$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -436,7 +437,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -461,7 +462,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0027-4676-9C29-CA1A8644F539}"/>
+              <c16:uniqueId val="{00000000-4701-4CA5-B079-156D33669683}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -750,7 +751,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$10</c:f>
+              <c:f>'v6'!$J$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -771,7 +772,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$11:$H$18</c:f>
+              <c:f>'v6'!$H$11:$H$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -804,7 +805,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$11:$J$18</c:f>
+              <c:f>'v6'!$J$11:$J$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -812,25 +813,836 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B574-44DC-9C51-C295C69082F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="637465960"/>
+        <c:axId val="637468256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="637465960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="637468256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="637468256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="637465960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>時間</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>phase0改変!$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>カウント</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>phase0改変!$D$11:$D$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>phase0改変!$F$11:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0027-4676-9C29-CA1A8644F539}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="626279792"/>
+        <c:axId val="626278808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="626279792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="626278808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="626278808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="626279792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>手数</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ja-JP"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>phase0改変!$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>カウント</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>phase0改変!$H$11:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52</c:v>
+                </c:pt>
                 <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>phase0改変!$J$11:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1124,6 +1936,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2130,7 +3022,1094 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3C89BE8-B36F-4A72-9EFE-353CA8566B72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{042BDC79-29DF-4E2B-8467-10AE038EDC9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2503,11 +4482,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F850FA3E-7370-4CAF-97C3-B834D7F59B04}">
-  <dimension ref="A1:J28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4653D650-7579-443F-970E-76983C1BDC78}">
+  <dimension ref="A1:J100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2521,6 +4500,12 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>3.498656988</v>
+      </c>
+      <c r="B2">
+        <v>53</v>
+      </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -2535,110 +4520,154 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>3.95343256</v>
+      </c>
+      <c r="B3">
+        <v>59</v>
+      </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="e">
+      <c r="E3">
         <f>AVERAGE(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" t="e">
+        <v>3.4081464922020199</v>
+      </c>
+      <c r="F3">
         <f>AVERAGE(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>56.707070707070706</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" t="e">
+      <c r="I3">
         <f>COUNTIFS(A:A,"&lt;10")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>96.969696969696969</v>
       </c>
       <c r="J3">
         <f>COUNT(B:B)</f>
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2.2160754200000001</v>
+      </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="e">
+      <c r="E4">
         <f>_xlfn.STDEV.S(A:A)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" t="e">
+        <v>2.3298548990780654</v>
+      </c>
+      <c r="F4">
         <f>_xlfn.STDEV.S(B:B)</f>
-        <v>#DIV/0!</v>
+        <v>2.2142973513635456</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="e">
+      <c r="I4">
         <f>COUNTIFS(A:A,"&lt;5")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>76.767676767676761</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>1.318476677</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5">
         <f>MAX(A:A)</f>
-        <v>0</v>
+        <v>11.615062</v>
       </c>
       <c r="F5">
         <f>MAX(B:B)</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" t="e">
+      <c r="I5">
         <f>COUNTIFS(A:A,"&lt;3")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>55.555555555555557</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>2.7343423370000002</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="e">
+      <c r="E6">
         <f>MEDIAN(A:A)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F6" t="e">
+        <v>2.7114114759999999</v>
+      </c>
+      <c r="F6">
         <f>MEDIAN(B:B)</f>
-        <v>#NUM!</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
-      <c r="I6" t="e">
+      <c r="I6">
         <f>COUNTIFS(A:A,"&lt;2")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>30.303030303030305</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>4.0348241329999999</v>
+      </c>
+      <c r="B7">
+        <v>57</v>
+      </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7">
         <f>MIN(A:A)</f>
-        <v>0</v>
+        <v>0.45532703400000002</v>
       </c>
       <c r="F7">
         <f>MIN(B:B)</f>
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="e">
+      <c r="I7">
         <f>COUNTIFS(A:A,"&lt;1")/COUNT(A:A)*100</f>
-        <v>#DIV/0!</v>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>4.0664949420000003</v>
+      </c>
+      <c r="B8">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>1.5445640089999999</v>
+      </c>
+      <c r="B9">
+        <v>56</v>
+      </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -2647,6 +4676,12 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>0.45532703400000002</v>
+      </c>
+      <c r="B10">
+        <v>52</v>
+      </c>
       <c r="D10" t="s">
         <v>14</v>
       </c>
@@ -2667,6 +4702,12 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>2.7807400229999999</v>
+      </c>
+      <c r="B11">
+        <v>57</v>
+      </c>
       <c r="D11">
         <v>0</v>
       </c>
@@ -2675,7 +4716,7 @@
       </c>
       <c r="F11">
         <f>COUNTIFS(A:A,"&lt;"&amp;E11,A:A,"&gt;="&amp;D11)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H11">
         <v>48</v>
@@ -2689,6 +4730,12 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>6.8871879580000002</v>
+      </c>
+      <c r="B12">
+        <v>58</v>
+      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -2697,7 +4744,7 @@
       </c>
       <c r="F12">
         <f t="shared" ref="F12:F27" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -2707,10 +4754,16 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>4.3709588049999999</v>
+      </c>
+      <c r="B13">
+        <v>57</v>
+      </c>
       <c r="D13">
         <v>2</v>
       </c>
@@ -2719,7 +4772,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H13">
         <v>52</v>
@@ -2729,10 +4782,16 @@
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>5.0908093450000003</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
       <c r="D14">
         <v>3</v>
       </c>
@@ -2741,7 +4800,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H14">
         <v>54</v>
@@ -2751,10 +4810,16 @@
       </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2.7114114759999999</v>
+      </c>
+      <c r="B15">
+        <v>54</v>
+      </c>
       <c r="D15">
         <v>4</v>
       </c>
@@ -2763,7 +4828,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <v>56</v>
@@ -2773,10 +4838,16 @@
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>4.268083334</v>
+      </c>
+      <c r="B16">
+        <v>58</v>
+      </c>
       <c r="D16">
         <v>5</v>
       </c>
@@ -2785,7 +4856,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H16">
         <v>58</v>
@@ -2795,10 +4866,16 @@
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>11.482353209999999</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
       <c r="D17">
         <v>6</v>
       </c>
@@ -2807,7 +4884,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H17">
         <v>60</v>
@@ -2817,10 +4894,16 @@
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>1.663481236</v>
+      </c>
+      <c r="B18">
+        <v>60</v>
+      </c>
       <c r="D18">
         <v>7</v>
       </c>
@@ -2829,7 +4912,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <v>62</v>
@@ -2839,10 +4922,16 @@
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>2.520831823</v>
+      </c>
+      <c r="B19">
+        <v>56</v>
+      </c>
       <c r="D19">
         <v>8</v>
       </c>
@@ -2851,10 +4940,16 @@
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>2.7624554630000002</v>
+      </c>
+      <c r="B20">
+        <v>56</v>
+      </c>
       <c r="D20">
         <v>9</v>
       </c>
@@ -2866,7 +4961,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>2.1642565729999999</v>
+      </c>
+      <c r="B21">
+        <v>55</v>
+      </c>
       <c r="D21">
         <v>10</v>
       </c>
@@ -2878,7 +4979,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>0.92003297799999995</v>
+      </c>
+      <c r="B22">
+        <v>51</v>
+      </c>
       <c r="D22">
         <v>11</v>
       </c>
@@ -2887,10 +4994,16 @@
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>5.2876226900000001</v>
+      </c>
+      <c r="B23">
+        <v>62</v>
+      </c>
       <c r="D23">
         <v>12</v>
       </c>
@@ -2902,7 +5015,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>1.47609067</v>
+      </c>
+      <c r="B24">
+        <v>54</v>
+      </c>
       <c r="D24">
         <v>13</v>
       </c>
@@ -2914,7 +5033,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>3.3785605429999999</v>
+      </c>
+      <c r="B25">
+        <v>58</v>
+      </c>
       <c r="D25">
         <v>14</v>
       </c>
@@ -2926,7 +5051,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>0.55252218200000003</v>
+      </c>
+      <c r="B26">
+        <v>56</v>
+      </c>
       <c r="D26">
         <v>15</v>
       </c>
@@ -2938,7 +5069,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>2.4374461169999999</v>
+      </c>
+      <c r="B27">
+        <v>56</v>
+      </c>
       <c r="D27">
         <v>16</v>
       </c>
@@ -2950,7 +5087,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>4.0292160509999997</v>
+      </c>
+      <c r="B28">
+        <v>59</v>
+      </c>
       <c r="D28">
         <v>17</v>
       </c>
@@ -2960,6 +5103,1789 @@
       <c r="F28">
         <f>COUNTIFS(A:A,"&lt;"&amp;E28,A:A,"&gt;="&amp;D28)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>3.0009808539999998</v>
+      </c>
+      <c r="B29">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>5.0973737239999997</v>
+      </c>
+      <c r="B30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>0.930514336</v>
+      </c>
+      <c r="B31">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>5.4481542110000003</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>6.795773745</v>
+      </c>
+      <c r="B33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>1.432799339</v>
+      </c>
+      <c r="B34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>3.542373419</v>
+      </c>
+      <c r="B35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>4.4916579719999996</v>
+      </c>
+      <c r="B36">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>1.493222952</v>
+      </c>
+      <c r="B37">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>0.97648549100000004</v>
+      </c>
+      <c r="B38">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>2.4919900890000002</v>
+      </c>
+      <c r="B39">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>1.169975996</v>
+      </c>
+      <c r="B40">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>3.403088093</v>
+      </c>
+      <c r="B41">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>2.0267639160000002</v>
+      </c>
+      <c r="B42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>1.080751896</v>
+      </c>
+      <c r="B43">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>0.75897049900000002</v>
+      </c>
+      <c r="B44">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>8.4923095699999998</v>
+      </c>
+      <c r="B45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>3.2616147990000002</v>
+      </c>
+      <c r="B46">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>11.343834879999999</v>
+      </c>
+      <c r="B47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>4.9565641879999998</v>
+      </c>
+      <c r="B48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>2.6487419609999998</v>
+      </c>
+      <c r="B49">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>11.615062</v>
+      </c>
+      <c r="B50">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>0.58245706600000002</v>
+      </c>
+      <c r="B51">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>5.5010030270000003</v>
+      </c>
+      <c r="B52">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>2.2674331670000001</v>
+      </c>
+      <c r="B53">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>2.8268525599999998</v>
+      </c>
+      <c r="B54">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>2.6159658430000001</v>
+      </c>
+      <c r="B55">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>2.5562233920000001</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>3.2133619790000001</v>
+      </c>
+      <c r="B57">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>0.84977388399999998</v>
+      </c>
+      <c r="B58">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>5.4424583909999997</v>
+      </c>
+      <c r="B59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>4.0240476129999996</v>
+      </c>
+      <c r="B60">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>2.3477466109999998</v>
+      </c>
+      <c r="B61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>6.1262435909999997</v>
+      </c>
+      <c r="B62">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>1.0591690540000001</v>
+      </c>
+      <c r="B63">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>1.3344326019999999</v>
+      </c>
+      <c r="B64">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>4.9881074429999996</v>
+      </c>
+      <c r="B65">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>5.0735111240000004</v>
+      </c>
+      <c r="B66">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>2.173287153</v>
+      </c>
+      <c r="B67">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>1.786780357</v>
+      </c>
+      <c r="B68">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>4.9256117340000003</v>
+      </c>
+      <c r="B69">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>5.4640052319999999</v>
+      </c>
+      <c r="B70">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>2.6988282200000002</v>
+      </c>
+      <c r="B71">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>1.9394247529999999</v>
+      </c>
+      <c r="B72">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>1.4936845299999999</v>
+      </c>
+      <c r="B73">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>4.0274057389999998</v>
+      </c>
+      <c r="B74">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>1.1968441009999999</v>
+      </c>
+      <c r="B75">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>1.8670947550000001</v>
+      </c>
+      <c r="B76">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>2.0175654889999999</v>
+      </c>
+      <c r="B77">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>6.6991634370000002</v>
+      </c>
+      <c r="B78">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>6.9386739730000002</v>
+      </c>
+      <c r="B79">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>3.5295660500000001</v>
+      </c>
+      <c r="B80">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>6.394960642</v>
+      </c>
+      <c r="B81">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>5.5737829210000003</v>
+      </c>
+      <c r="B82">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>2.6938018800000001</v>
+      </c>
+      <c r="B83">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>1.489348173</v>
+      </c>
+      <c r="B84">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>5.21873641</v>
+      </c>
+      <c r="B85">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>2.7208981510000001</v>
+      </c>
+      <c r="B86">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>2.6389462950000002</v>
+      </c>
+      <c r="B87">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>1.887147903</v>
+      </c>
+      <c r="B88">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>1.1079926490000001</v>
+      </c>
+      <c r="B89">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>6.5557498929999998</v>
+      </c>
+      <c r="B90">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>2.0838229660000001</v>
+      </c>
+      <c r="B91">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>2.5241093640000001</v>
+      </c>
+      <c r="B92">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>1.2945413589999999</v>
+      </c>
+      <c r="B93">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>2.0090491770000001</v>
+      </c>
+      <c r="B94">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>4.6146523950000002</v>
+      </c>
+      <c r="B95">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>5.0910081859999998</v>
+      </c>
+      <c r="B96">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97">
+        <v>7.2314622399999999</v>
+      </c>
+      <c r="B97">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A98">
+        <v>1.139464617</v>
+      </c>
+      <c r="B98">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A99">
+        <v>0.90886139899999996</v>
+      </c>
+      <c r="B99">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A100">
+        <v>1.5961847309999999</v>
+      </c>
+      <c r="B100">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F850FA3E-7370-4CAF-97C3-B834D7F59B04}">
+  <dimension ref="A1:J100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2.0565037730000002</v>
+      </c>
+      <c r="B2">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2.3667221070000002</v>
+      </c>
+      <c r="B3">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(A:A)</f>
+        <v>4.3407332006666666</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(B:B)</f>
+        <v>57.454545454545453</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <f>COUNTIFS(A:A,"&lt;10")/COUNT(A:A)*100</f>
+        <v>94.949494949494948</v>
+      </c>
+      <c r="J3">
+        <f>COUNT(B:B)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>7.1883742809999998</v>
+      </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f>_xlfn.STDEV.S(A:A)</f>
+        <v>3.1669576428023527</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.STDEV.S(B:B)</f>
+        <v>2.086265716110709</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <f>COUNTIFS(A:A,"&lt;5")/COUNT(A:A)*100</f>
+        <v>68.686868686868678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>9.1296842100000006</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <f>MAX(A:A)</f>
+        <v>18.214314940000001</v>
+      </c>
+      <c r="F5">
+        <f>MAX(B:B)</f>
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <f>COUNTIFS(A:A,"&lt;3")/COUNT(A:A)*100</f>
+        <v>44.444444444444443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>2.4662380220000002</v>
+      </c>
+      <c r="B6">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f>MEDIAN(A:A)</f>
+        <v>3.5675737860000001</v>
+      </c>
+      <c r="F6">
+        <f>MEDIAN(B:B)</f>
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <f>COUNTIFS(A:A,"&lt;2")/COUNT(A:A)*100</f>
+        <v>21.212121212121211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>4.8123106959999999</v>
+      </c>
+      <c r="B7">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <f>MIN(A:A)</f>
+        <v>0.60938406000000001</v>
+      </c>
+      <c r="F7">
+        <f>MIN(B:B)</f>
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7">
+        <f>COUNTIFS(A:A,"&lt;1")/COUNT(A:A)*100</f>
+        <v>1.0101010101010102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>2.882128716</v>
+      </c>
+      <c r="B8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>2.6736319069999999</v>
+      </c>
+      <c r="B9">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>1.945328712</v>
+      </c>
+      <c r="B10">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>9.0379238130000008</v>
+      </c>
+      <c r="B11">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>COUNTIFS(A:A,"&lt;"&amp;E11,A:A,"&gt;="&amp;D11)</f>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>48</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J18" si="0">COUNTIFS(B:B,"&lt;"&amp;I11,B:B,"&gt;="&amp;H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>4.8975746630000003</v>
+      </c>
+      <c r="B12">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F27" si="1">COUNTIFS(A:A,"&lt;"&amp;E12,A:A,"&gt;="&amp;D12)</f>
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>52</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>3.5345528129999999</v>
+      </c>
+      <c r="B13">
+        <v>57</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>52</v>
+      </c>
+      <c r="I13">
+        <v>54</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>10.5059247</v>
+      </c>
+      <c r="B14">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>54</v>
+      </c>
+      <c r="I14">
+        <v>56</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>2.1857166289999999</v>
+      </c>
+      <c r="B15">
+        <v>56</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>56</v>
+      </c>
+      <c r="I15">
+        <v>58</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>3.1460089679999999</v>
+      </c>
+      <c r="B16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>58</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>4.5508470540000001</v>
+      </c>
+      <c r="B17">
+        <v>59</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>60</v>
+      </c>
+      <c r="I17">
+        <v>62</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>1.539812803</v>
+      </c>
+      <c r="B18">
+        <v>56</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>62</v>
+      </c>
+      <c r="I18">
+        <v>64</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>17.818089010000001</v>
+      </c>
+      <c r="B19">
+        <v>55</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>6.311275244</v>
+      </c>
+      <c r="B20">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>1.4890189170000001</v>
+      </c>
+      <c r="B21">
+        <v>57</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>7.1194791789999998</v>
+      </c>
+      <c r="B22">
+        <v>57</v>
+      </c>
+      <c r="D22">
+        <v>11</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>1.050193071</v>
+      </c>
+      <c r="B23">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>13</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>1.3005230430000001</v>
+      </c>
+      <c r="B24">
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>13</v>
+      </c>
+      <c r="E24">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>2.6309688090000001</v>
+      </c>
+      <c r="B25">
+        <v>57</v>
+      </c>
+      <c r="D25">
+        <v>14</v>
+      </c>
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>5.5142612460000002</v>
+      </c>
+      <c r="B26">
+        <v>59</v>
+      </c>
+      <c r="D26">
+        <v>15</v>
+      </c>
+      <c r="E26">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>5.1493916510000002</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>17</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28">
+        <v>7.094502211</v>
+      </c>
+      <c r="B28">
+        <v>58</v>
+      </c>
+      <c r="D28">
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>18</v>
+      </c>
+      <c r="F28">
+        <f>COUNTIFS(A:A,"&lt;"&amp;E28,A:A,"&gt;="&amp;D28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>1.871587753</v>
+      </c>
+      <c r="B29">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>4.7004361149999996</v>
+      </c>
+      <c r="B30">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>2.1332976819999998</v>
+      </c>
+      <c r="B31">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>5.4813499449999998</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>0.60938406000000001</v>
+      </c>
+      <c r="B33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>4.0342230800000003</v>
+      </c>
+      <c r="B34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>2.8493831159999998</v>
+      </c>
+      <c r="B35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>2.6497013570000001</v>
+      </c>
+      <c r="B36">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>3.5138146880000001</v>
+      </c>
+      <c r="B37">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>5.5368165969999996</v>
+      </c>
+      <c r="B38">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39">
+        <v>6.8143084050000002</v>
+      </c>
+      <c r="B39">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40">
+        <v>2.8374094959999998</v>
+      </c>
+      <c r="B40">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41">
+        <v>2.4824323650000002</v>
+      </c>
+      <c r="B41">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42">
+        <v>3.6488964560000001</v>
+      </c>
+      <c r="B42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43">
+        <v>3.8045988080000002</v>
+      </c>
+      <c r="B43">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44">
+        <v>4.9397971629999997</v>
+      </c>
+      <c r="B44">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45">
+        <v>8.406528711</v>
+      </c>
+      <c r="B45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46">
+        <v>1.5997245309999999</v>
+      </c>
+      <c r="B46">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47">
+        <v>4.1568896769999997</v>
+      </c>
+      <c r="B47">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48">
+        <v>1.9088945390000001</v>
+      </c>
+      <c r="B48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49">
+        <v>4.2695875169999997</v>
+      </c>
+      <c r="B49">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50">
+        <v>18.214314940000001</v>
+      </c>
+      <c r="B50">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51">
+        <v>5.6449465749999996</v>
+      </c>
+      <c r="B51">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52">
+        <v>1.080109835</v>
+      </c>
+      <c r="B52">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>1.8156533239999999</v>
+      </c>
+      <c r="B53">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>11.748306749999999</v>
+      </c>
+      <c r="B54">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>2.4495034219999998</v>
+      </c>
+      <c r="B55">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>3.7406306269999998</v>
+      </c>
+      <c r="B56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57">
+        <v>4.1194784640000002</v>
+      </c>
+      <c r="B57">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58">
+        <v>2.932047367</v>
+      </c>
+      <c r="B58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59">
+        <v>5.3541896339999999</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60">
+        <v>6.0878844259999996</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61">
+        <v>3.477242231</v>
+      </c>
+      <c r="B61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62">
+        <v>1.882935762</v>
+      </c>
+      <c r="B62">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63">
+        <v>4.6237931249999997</v>
+      </c>
+      <c r="B63">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64">
+        <v>2.3407170769999999</v>
+      </c>
+      <c r="B64">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65">
+        <v>6.1316978930000001</v>
+      </c>
+      <c r="B65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66">
+        <v>2.76168251</v>
+      </c>
+      <c r="B66">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67">
+        <v>2.3119978899999998</v>
+      </c>
+      <c r="B67">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68">
+        <v>5.2517769339999996</v>
+      </c>
+      <c r="B68">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69">
+        <v>13.38240886</v>
+      </c>
+      <c r="B69">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70">
+        <v>6.8553612230000001</v>
+      </c>
+      <c r="B70">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71">
+        <v>5.9494686129999996</v>
+      </c>
+      <c r="B71">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72">
+        <v>2.5666737560000001</v>
+      </c>
+      <c r="B72">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73">
+        <v>2.5204219819999998</v>
+      </c>
+      <c r="B73">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74">
+        <v>1.61705637</v>
+      </c>
+      <c r="B74">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A75">
+        <v>1.027253151</v>
+      </c>
+      <c r="B75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A76">
+        <v>5.477518559</v>
+      </c>
+      <c r="B76">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A77">
+        <v>6.9086916450000002</v>
+      </c>
+      <c r="B77">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A78">
+        <v>4.681096792</v>
+      </c>
+      <c r="B78">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A79">
+        <v>1.1210625169999999</v>
+      </c>
+      <c r="B79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A80">
+        <v>1.9197716709999999</v>
+      </c>
+      <c r="B80">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A81">
+        <v>3.8817250730000001</v>
+      </c>
+      <c r="B81">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82">
+        <v>4.3266217710000001</v>
+      </c>
+      <c r="B82">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A83">
+        <v>2.467030287</v>
+      </c>
+      <c r="B83">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84">
+        <v>5.2842516899999996</v>
+      </c>
+      <c r="B84">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A85">
+        <v>1.580489874</v>
+      </c>
+      <c r="B85">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A86">
+        <v>3.4741928579999999</v>
+      </c>
+      <c r="B86">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A87">
+        <v>1.4342393879999999</v>
+      </c>
+      <c r="B87">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A88">
+        <v>3.5675737860000001</v>
+      </c>
+      <c r="B88">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A89">
+        <v>2.097951412</v>
+      </c>
+      <c r="B89">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A90">
+        <v>1.20652914</v>
+      </c>
+      <c r="B90">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A91">
+        <v>4.9439413549999998</v>
+      </c>
+      <c r="B91">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A92">
+        <v>3.6958558560000001</v>
+      </c>
+      <c r="B92">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A93">
+        <v>5.9438953400000001</v>
+      </c>
+      <c r="B93">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A94">
+        <v>9.2828667159999991</v>
+      </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A95">
+        <v>8.2643628119999999</v>
+      </c>
+      <c r="B95">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A96">
+        <v>2.8810472489999999</v>
+      </c>
+      <c r="B96">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97">
+        <v>2.1027204990000001</v>
+      </c>
+      <c r="B97">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A98">
+        <v>1.1155776980000001</v>
+      </c>
+      <c r="B98">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A99">
+        <v>1.872080564</v>
+      </c>
+      <c r="B99">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A100">
+        <v>5.6678912639999997</v>
+      </c>
+      <c r="B100">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>